<commit_message>
relaced Kcat with the correct name Km in Henri-Michaelis-Menten reactions
</commit_message>
<xml_diff>
--- a/Viswan_2018.xlsx
+++ b/Viswan_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Viswan_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36898C4C-0BEC-430F-9C5F-A043CCDFCE36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BE707C-EBA5-41D7-891C-9ED7E570319E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="2220" windowWidth="28800" windowHeight="15472" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="27045" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="13" r:id="rId1"/>
@@ -3686,22 +3686,22 @@
     <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='E1I' TableTitle='Viswan_2018 E1I' TableType = 'QuantityMatrix'</t>
   </si>
   <si>
-    <t>(Vmax_R86*PIP2*Ca_PLC_g_p/(Kcat_R86+PIP2))</t>
-  </si>
-  <si>
-    <t>(Vmax_R85*PIP2*Ca_PLC_g/(Kcat_R85+PIP2))</t>
-  </si>
-  <si>
-    <t>Kcat_R85</t>
-  </si>
-  <si>
-    <t>Kcat_R86</t>
-  </si>
-  <si>
     <t>Vmax_R85</t>
   </si>
   <si>
     <t>Vmax_R86</t>
+  </si>
+  <si>
+    <t>(Vmax_R85*PIP2*Ca_PLC_g/(Km_R85+PIP2))</t>
+  </si>
+  <si>
+    <t>(Vmax_R86*PIP2*Ca_PLC_g_p/(Km_R86+PIP2))</t>
+  </si>
+  <si>
+    <t>Km_R85</t>
+  </si>
+  <si>
+    <t>Km_R86</t>
   </si>
 </sst>
 </file>
@@ -4444,7 +4444,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7771,8 +7771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12454,7 +12454,7 @@
         <v>616</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>224</v>
@@ -12489,7 +12489,7 @@
         <v>618</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>1192</v>
@@ -12524,7 +12524,7 @@
         <v>620</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>224</v>
@@ -12559,7 +12559,7 @@
         <v>622</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>1192</v>
@@ -13440,8 +13440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87:D88"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15509,7 +15509,7 @@
         <v>1038</v>
       </c>
       <c r="C87" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D87" t="b">
         <f>FALSE()</f>
@@ -15533,7 +15533,7 @@
         <v>1042</v>
       </c>
       <c r="C88" t="s">
-        <v>1214</v>
+        <v>1217</v>
       </c>
       <c r="D88" t="b">
         <f>FALSE()</f>

</xml_diff>